<commit_message>
Finish all function + added 2 remaining companies' data
</commit_message>
<xml_diff>
--- a/financial_data/result.xlsx
+++ b/financial_data/result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4268" uniqueCount="1370">
   <si>
     <t>Mô ta biến:</t>
   </si>
@@ -2922,6 +2922,1218 @@
   </si>
   <si>
     <t>28984859151</t>
+  </si>
+  <si>
+    <t>122010</t>
+  </si>
+  <si>
+    <t>511844617258</t>
+  </si>
+  <si>
+    <t>247412110960</t>
+  </si>
+  <si>
+    <t>230402292148</t>
+  </si>
+  <si>
+    <t>244021480342</t>
+  </si>
+  <si>
+    <t>235758703264</t>
+  </si>
+  <si>
+    <t>442042619077</t>
+  </si>
+  <si>
+    <t>373619014357</t>
+  </si>
+  <si>
+    <t>313823478523</t>
+  </si>
+  <si>
+    <t>85000000000</t>
+  </si>
+  <si>
+    <t>94977301397</t>
+  </si>
+  <si>
+    <t>792186837777</t>
+  </si>
+  <si>
+    <t>780739788443</t>
+  </si>
+  <si>
+    <t>473477940816</t>
+  </si>
+  <si>
+    <t>46084766631</t>
+  </si>
+  <si>
+    <t>22488640000</t>
+  </si>
+  <si>
+    <t>81577608848</t>
+  </si>
+  <si>
+    <t>9597</t>
+  </si>
+  <si>
+    <t>11447049334</t>
+  </si>
+  <si>
+    <t>122011</t>
+  </si>
+  <si>
+    <t>610954451564</t>
+  </si>
+  <si>
+    <t>7033880977</t>
+  </si>
+  <si>
+    <t>7033 880977</t>
+  </si>
+  <si>
+    <t>315420045025</t>
+  </si>
+  <si>
+    <t>245035133831</t>
+  </si>
+  <si>
+    <t>238873314292</t>
+  </si>
+  <si>
+    <t>230544848072</t>
+  </si>
+  <si>
+    <t>849827765856</t>
+  </si>
+  <si>
+    <t>482428575975</t>
+  </si>
+  <si>
+    <t>454496943728</t>
+  </si>
+  <si>
+    <t>367399189881</t>
+  </si>
+  <si>
+    <t>109243949362</t>
+  </si>
+  <si>
+    <t>868061769552</t>
+  </si>
+  <si>
+    <t>851234055137</t>
+  </si>
+  <si>
+    <t>407262447052</t>
+  </si>
+  <si>
+    <t>49843118503</t>
+  </si>
+  <si>
+    <t>34411910765</t>
+  </si>
+  <si>
+    <t>96696937650</t>
+  </si>
+  <si>
+    <t>16827714415</t>
+  </si>
+  <si>
+    <t>752730495991</t>
+  </si>
+  <si>
+    <t>8561114404</t>
+  </si>
+  <si>
+    <t>370141420316</t>
+  </si>
+  <si>
+    <t>337029686140</t>
+  </si>
+  <si>
+    <t>237037643289</t>
+  </si>
+  <si>
+    <t>217245774295</t>
+  </si>
+  <si>
+    <t>511102701876</t>
+  </si>
+  <si>
+    <t>505341970862</t>
+  </si>
+  <si>
+    <t>478665437404</t>
+  </si>
+  <si>
+    <t>89200000000</t>
+  </si>
+  <si>
+    <t>134038860076</t>
+  </si>
+  <si>
+    <t>1024001149566</t>
+  </si>
+  <si>
+    <t>1010693544332</t>
+  </si>
+  <si>
+    <t>486159567797</t>
+  </si>
+  <si>
+    <t>44142541838</t>
+  </si>
+  <si>
+    <t>42053632256</t>
+  </si>
+  <si>
+    <t>48253324733</t>
+  </si>
+  <si>
+    <t>122677281125</t>
+  </si>
+  <si>
+    <t>14140</t>
+  </si>
+  <si>
+    <t>13307605234</t>
+  </si>
+  <si>
+    <t>847434432294</t>
+  </si>
+  <si>
+    <t>88815365469</t>
+  </si>
+  <si>
+    <t>38815365469</t>
+  </si>
+  <si>
+    <t>397492287926</t>
+  </si>
+  <si>
+    <t>335621883187</t>
+  </si>
+  <si>
+    <t>233714218740</t>
+  </si>
+  <si>
+    <t>215323126389</t>
+  </si>
+  <si>
+    <t>383224564626</t>
+  </si>
+  <si>
+    <t>353087964626</t>
+  </si>
+  <si>
+    <t>697924086408</t>
+  </si>
+  <si>
+    <t>178400000000</t>
+  </si>
+  <si>
+    <t>187086226591</t>
+  </si>
+  <si>
+    <t>1207805355127</t>
+  </si>
+  <si>
+    <t>1188030523144</t>
+  </si>
+  <si>
+    <t>572788750670</t>
+  </si>
+  <si>
+    <t>30073766663</t>
+  </si>
+  <si>
+    <t>23630618885</t>
+  </si>
+  <si>
+    <t>43353432928</t>
+  </si>
+  <si>
+    <t>148460241173</t>
+  </si>
+  <si>
+    <t>15738</t>
+  </si>
+  <si>
+    <t>19774831983</t>
+  </si>
+  <si>
+    <t>919606072423</t>
+  </si>
+  <si>
+    <t>107423680889</t>
+  </si>
+  <si>
+    <t>27423680889</t>
+  </si>
+  <si>
+    <t>397182787727</t>
+  </si>
+  <si>
+    <t>370249501716</t>
+  </si>
+  <si>
+    <t>240040525633</t>
+  </si>
+  <si>
+    <t>216031438371</t>
+  </si>
+  <si>
+    <t>253359562123</t>
+  </si>
+  <si>
+    <t>215418462123</t>
+  </si>
+  <si>
+    <t>906287035933</t>
+  </si>
+  <si>
+    <t>267600000000</t>
+  </si>
+  <si>
+    <t>190168345342</t>
+  </si>
+  <si>
+    <t>1171998652336</t>
+  </si>
+  <si>
+    <t>1148558662932</t>
+  </si>
+  <si>
+    <t>581197580573</t>
+  </si>
+  <si>
+    <t>10143169581</t>
+  </si>
+  <si>
+    <t>4659667520</t>
+  </si>
+  <si>
+    <t>41928992467</t>
+  </si>
+  <si>
+    <t>148149853143</t>
+  </si>
+  <si>
+    <t>7792</t>
+  </si>
+  <si>
+    <t>23439989404</t>
+  </si>
+  <si>
+    <t>1007147961001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">244462733921 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39462733921 
+</t>
+  </si>
+  <si>
+    <t>80000000000</t>
+  </si>
+  <si>
+    <t>382207045492</t>
+  </si>
+  <si>
+    <t>278262420827</t>
+  </si>
+  <si>
+    <t>369041036793</t>
+  </si>
+  <si>
+    <t>327427547834</t>
+  </si>
+  <si>
+    <t>287770932445</t>
+  </si>
+  <si>
+    <t>247496332445</t>
+  </si>
+  <si>
+    <t>1088418065349</t>
+  </si>
+  <si>
+    <t>401400000000</t>
+  </si>
+  <si>
+    <t>229909174572</t>
+  </si>
+  <si>
+    <t>1344805397319</t>
+  </si>
+  <si>
+    <t>1308505542154</t>
+  </si>
+  <si>
+    <t>684357451795</t>
+  </si>
+  <si>
+    <t>8944233426</t>
+  </si>
+  <si>
+    <t>2157000000</t>
+  </si>
+  <si>
+    <t>349298260913</t>
+  </si>
+  <si>
+    <t>41312821481</t>
+  </si>
+  <si>
+    <t>183612527947</t>
+  </si>
+  <si>
+    <t>5680 DN:4409</t>
+  </si>
+  <si>
+    <t>36299855165</t>
+  </si>
+  <si>
+    <t>1253811555161</t>
+  </si>
+  <si>
+    <t>77069898988</t>
+  </si>
+  <si>
+    <t>37069898988</t>
+  </si>
+  <si>
+    <t>419491925621</t>
+  </si>
+  <si>
+    <t>304986619443</t>
+  </si>
+  <si>
+    <t>367307128571</t>
+  </si>
+  <si>
+    <t>304726293095</t>
+  </si>
+  <si>
+    <t>294942039718</t>
+  </si>
+  <si>
+    <t>246025039718</t>
+  </si>
+  <si>
+    <t>1326176644014</t>
+  </si>
+  <si>
+    <t>501750000000</t>
+  </si>
+  <si>
+    <t>299911683899</t>
+  </si>
+  <si>
+    <t>1538279873742</t>
+  </si>
+  <si>
+    <t>1507961143465</t>
+  </si>
+  <si>
+    <t>788187698499</t>
+  </si>
+  <si>
+    <t>7639010683</t>
+  </si>
+  <si>
+    <t>386019190335</t>
+  </si>
+  <si>
+    <t>50119170665</t>
+  </si>
+  <si>
+    <t>239258578665</t>
+  </si>
+  <si>
+    <t>5136</t>
+  </si>
+  <si>
+    <t>30318730277</t>
+  </si>
+  <si>
+    <t>1597850438405</t>
+  </si>
+  <si>
+    <t>42582580492</t>
+  </si>
+  <si>
+    <t>635000000000</t>
+  </si>
+  <si>
+    <t>471761468229</t>
+  </si>
+  <si>
+    <t>400000217738</t>
+  </si>
+  <si>
+    <t>358087048287</t>
+  </si>
+  <si>
+    <t>285903789344</t>
+  </si>
+  <si>
+    <t>346329830714</t>
+  </si>
+  <si>
+    <t>304239652381</t>
+  </si>
+  <si>
+    <t>1609607655978</t>
+  </si>
+  <si>
+    <t>652275000000</t>
+  </si>
+  <si>
+    <t>358911012879</t>
+  </si>
+  <si>
+    <t>1655108694444</t>
+  </si>
+  <si>
+    <t>1622353239322</t>
+  </si>
+  <si>
+    <t>841736445654</t>
+  </si>
+  <si>
+    <t>8113705428</t>
+  </si>
+  <si>
+    <t>396533258294</t>
+  </si>
+  <si>
+    <t>54057372527</t>
+  </si>
+  <si>
+    <t>286431011964</t>
+  </si>
+  <si>
+    <t>4984</t>
+  </si>
+  <si>
+    <t>32755455122</t>
+  </si>
+  <si>
+    <t>1711319846321</t>
+  </si>
+  <si>
+    <t>357245509279</t>
+  </si>
+  <si>
+    <t>96245509279</t>
+  </si>
+  <si>
+    <t>189000000000</t>
+  </si>
+  <si>
+    <t>480614083624</t>
+  </si>
+  <si>
+    <t>450110824303</t>
+  </si>
+  <si>
+    <t>422023118657</t>
+  </si>
+  <si>
+    <t>2133342964978</t>
+  </si>
+  <si>
+    <t>347812611982</t>
+  </si>
+  <si>
+    <t>315978853649</t>
+  </si>
+  <si>
+    <t>1785530352996</t>
+  </si>
+  <si>
+    <t>750116250000</t>
+  </si>
+  <si>
+    <t>386480428681</t>
+  </si>
+  <si>
+    <t>1711291180125</t>
+  </si>
+  <si>
+    <t>1674848940759</t>
+  </si>
+  <si>
+    <t>868268763818</t>
+  </si>
+  <si>
+    <t>307872357467</t>
+  </si>
+  <si>
+    <t>2087400000 
+391816568192</t>
+  </si>
+  <si>
+    <t>54839551083</t>
+  </si>
+  <si>
+    <t>309377697018</t>
+  </si>
+  <si>
+    <t>4084</t>
+  </si>
+  <si>
+    <t>36442239366</t>
+  </si>
+  <si>
+    <t>1226340165317</t>
+  </si>
+  <si>
+    <t>60328276222</t>
+  </si>
+  <si>
+    <t>611350261974</t>
+  </si>
+  <si>
+    <t>518384645657</t>
+  </si>
+  <si>
+    <t>1075507428552</t>
+  </si>
+  <si>
+    <t>298067182010</t>
+  </si>
+  <si>
+    <t>2301847593869</t>
+  </si>
+  <si>
+    <t>347381560271</t>
+  </si>
+  <si>
+    <t>326443414175</t>
+  </si>
+  <si>
+    <t>1954466033598</t>
+  </si>
+  <si>
+    <t>401816404955</t>
+  </si>
+  <si>
+    <t>1885370505023</t>
+  </si>
+  <si>
+    <t>1846923436433</t>
+  </si>
+  <si>
+    <t>1021630484006</t>
+  </si>
+  <si>
+    <t>8678922 100</t>
+  </si>
+  <si>
+    <t>2572 798 128</t>
+  </si>
+  <si>
+    <t>363438822041</t>
+  </si>
+  <si>
+    <t>62016667072</t>
+  </si>
+  <si>
+    <t>320958930602</t>
+  </si>
+  <si>
+    <t>4252</t>
+  </si>
+  <si>
+    <t>38447068590</t>
+  </si>
+  <si>
+    <t>1414546592868</t>
+  </si>
+  <si>
+    <t>30681435370</t>
+  </si>
+  <si>
+    <t>814554438458</t>
+  </si>
+  <si>
+    <t>1148311786245</t>
+  </si>
+  <si>
+    <t>2562858379113</t>
+  </si>
+  <si>
+    <t>517382677425</t>
+  </si>
+  <si>
+    <t>507818267294</t>
+  </si>
+  <si>
+    <t>125971941806</t>
+  </si>
+  <si>
+    <t>2045475701688</t>
+  </si>
+  <si>
+    <t>750 116250000</t>
+  </si>
+  <si>
+    <t>397781194239</t>
+  </si>
+  <si>
+    <t>2036797867896</t>
+  </si>
+  <si>
+    <t>1934277133563</t>
+  </si>
+  <si>
+    <t>1097837462225</t>
+  </si>
+  <si>
+    <t>15577001170</t>
+  </si>
+  <si>
+    <t>9081336420</t>
+  </si>
+  <si>
+    <t>368320781916</t>
+  </si>
+  <si>
+    <t>62133020538</t>
+  </si>
+  <si>
+    <t>317044543090</t>
+  </si>
+  <si>
+    <t>4213</t>
+  </si>
+  <si>
+    <t>102520734333</t>
+  </si>
+  <si>
+    <t>1593416129655</t>
+  </si>
+  <si>
+    <t>85646642074</t>
+  </si>
+  <si>
+    <t>777514588188</t>
+  </si>
+  <si>
+    <t>678653448597</t>
+  </si>
+  <si>
+    <t>1134518778053</t>
+  </si>
+  <si>
+    <t>1051574831350</t>
+  </si>
+  <si>
+    <t>2727934907708</t>
+  </si>
+  <si>
+    <t>668585804220</t>
+  </si>
+  <si>
+    <t>664435921830</t>
+  </si>
+  <si>
+    <t>205331581146</t>
+  </si>
+  <si>
+    <t>2059349103488</t>
+  </si>
+  <si>
+    <t>206120814750</t>
+  </si>
+  <si>
+    <t>1089755439217</t>
+  </si>
+  <si>
+    <t>1076344041102</t>
+  </si>
+  <si>
+    <t>643009918972</t>
+  </si>
+  <si>
+    <t>5763793620</t>
+  </si>
+  <si>
+    <t>164896651800</t>
+  </si>
+  <si>
+    <t>2192</t>
+  </si>
+  <si>
+    <t>13411398115</t>
+  </si>
+  <si>
+    <t>142125760340</t>
+  </si>
+  <si>
+    <t>8883654732</t>
+  </si>
+  <si>
+    <t>61643825081</t>
+  </si>
+  <si>
+    <t>21546790191</t>
+  </si>
+  <si>
+    <t>445910865771</t>
+  </si>
+  <si>
+    <t>222215398970</t>
+  </si>
+  <si>
+    <t>378404019679</t>
+  </si>
+  <si>
+    <t>277239449129</t>
+  </si>
+  <si>
+    <t>123161982929</t>
+  </si>
+  <si>
+    <t>209632606432</t>
+  </si>
+  <si>
+    <t>180000000000</t>
+  </si>
+  <si>
+    <t>10969115731</t>
+  </si>
+  <si>
+    <t>387083106688</t>
+  </si>
+  <si>
+    <t>377051497280</t>
+  </si>
+  <si>
+    <t>335771098243</t>
+  </si>
+  <si>
+    <t>8099031415</t>
+  </si>
+  <si>
+    <t>21557994784</t>
+  </si>
+  <si>
+    <t>7881428683</t>
+  </si>
+  <si>
+    <t>9364859130</t>
+  </si>
+  <si>
+    <t>530</t>
+  </si>
+  <si>
+    <t>10031609408</t>
+  </si>
+  <si>
+    <t>397990591490</t>
+  </si>
+  <si>
+    <t>31349149576</t>
+  </si>
+  <si>
+    <t>67150000000</t>
+  </si>
+  <si>
+    <t>31386433627</t>
+  </si>
+  <si>
+    <t>15458690377</t>
+  </si>
+  <si>
+    <t>579853112083</t>
+  </si>
+  <si>
+    <t>30274560392</t>
+  </si>
+  <si>
+    <t>541617000575</t>
+  </si>
+  <si>
+    <t>386633452176</t>
+  </si>
+  <si>
+    <t>241298400000</t>
+  </si>
+  <si>
+    <t>436226702998</t>
+  </si>
+  <si>
+    <t>330000000000</t>
+  </si>
+  <si>
+    <t>32907158633</t>
+  </si>
+  <si>
+    <t>468923179068</t>
+  </si>
+  <si>
+    <t>447262868515</t>
+  </si>
+  <si>
+    <t>367366438235</t>
+  </si>
+  <si>
+    <t>18576862479</t>
+  </si>
+  <si>
+    <t>18526139729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44963985954 
+</t>
+  </si>
+  <si>
+    <t>19841776270</t>
+  </si>
+  <si>
+    <t>22428582579</t>
+  </si>
+  <si>
+    <t>1145</t>
+  </si>
+  <si>
+    <t>21660310553</t>
+  </si>
+  <si>
+    <t>271670499341</t>
+  </si>
+  <si>
+    <t>32628439242</t>
+  </si>
+  <si>
+    <t>32628 439242</t>
+  </si>
+  <si>
+    <t>138313514746</t>
+  </si>
+  <si>
+    <t>34268535845</t>
+  </si>
+  <si>
+    <t>1006506795826</t>
+  </si>
+  <si>
+    <t>207770893622</t>
+  </si>
+  <si>
+    <t>773251993661</t>
+  </si>
+  <si>
+    <t>522270791319</t>
+  </si>
+  <si>
+    <t>329701625563</t>
+  </si>
+  <si>
+    <t>504925301506</t>
+  </si>
+  <si>
+    <t>58263284640</t>
+  </si>
+  <si>
+    <t>919620002905</t>
+  </si>
+  <si>
+    <t>879723581279</t>
+  </si>
+  <si>
+    <t>727110771712</t>
+  </si>
+  <si>
+    <t>25470989565</t>
+  </si>
+  <si>
+    <t>25399701525</t>
+  </si>
+  <si>
+    <t>73927617361</t>
+  </si>
+  <si>
+    <t>24466574439</t>
+  </si>
+  <si>
+    <t>1480</t>
+  </si>
+  <si>
+    <t>39896421626</t>
+  </si>
+  <si>
+    <t>307458395731</t>
+  </si>
+  <si>
+    <t>36576431751</t>
+  </si>
+  <si>
+    <t>154235041876</t>
+  </si>
+  <si>
+    <t>13547914165</t>
+  </si>
+  <si>
+    <t>1011312405115</t>
+  </si>
+  <si>
+    <t>274093983905</t>
+  </si>
+  <si>
+    <t>843657991496</t>
+  </si>
+  <si>
+    <t>632721833310</t>
+  </si>
+  <si>
+    <t>472149323000</t>
+  </si>
+  <si>
+    <t>475112809350</t>
+  </si>
+  <si>
+    <t>379498470000</t>
+  </si>
+  <si>
+    <t>1258561038209</t>
+  </si>
+  <si>
+    <t>1211335888255</t>
+  </si>
+  <si>
+    <t>1006484568533</t>
+  </si>
+  <si>
+    <t>33655025844</t>
+  </si>
+  <si>
+    <t>33453161846</t>
+  </si>
+  <si>
+    <t>82415078022</t>
+  </si>
+  <si>
+    <t>31229059410</t>
+  </si>
+  <si>
+    <t>87187508347</t>
+  </si>
+  <si>
+    <t>226188</t>
+  </si>
+  <si>
+    <t>47225149954</t>
+  </si>
+  <si>
+    <t>415406202210</t>
+  </si>
+  <si>
+    <t>47033461532</t>
+  </si>
+  <si>
+    <t>251687303127</t>
+  </si>
+  <si>
+    <t>30052374596</t>
+  </si>
+  <si>
+    <t>1067529875700</t>
+  </si>
+  <si>
+    <t>591062763019</t>
+  </si>
+  <si>
+    <t>919713735591</t>
+  </si>
+  <si>
+    <t>724087076681</t>
+  </si>
+  <si>
+    <t>555729384160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">563222342319 
+</t>
+  </si>
+  <si>
+    <t>421240940000</t>
+  </si>
+  <si>
+    <t>83182957328</t>
+  </si>
+  <si>
+    <t>1400647668769</t>
+  </si>
+  <si>
+    <t>1359242852128</t>
+  </si>
+  <si>
+    <t>1111533521845</t>
+  </si>
+  <si>
+    <t>45196644767</t>
+  </si>
+  <si>
+    <t>45169454646</t>
+  </si>
+  <si>
+    <t>106559584344</t>
+  </si>
+  <si>
+    <t>30641627100</t>
+  </si>
+  <si>
+    <t>62109532969</t>
+  </si>
+  <si>
+    <t>1411</t>
+  </si>
+  <si>
+    <t>41404816641</t>
+  </si>
+  <si>
+    <t>359840852653</t>
+  </si>
+  <si>
+    <t>84051907860</t>
+  </si>
+  <si>
+    <t>175169014124</t>
+  </si>
+  <si>
+    <t>25578514868</t>
+  </si>
+  <si>
+    <t>1128800716151</t>
+  </si>
+  <si>
+    <t>554478555416</t>
+  </si>
+  <si>
+    <t>699067263065</t>
+  </si>
+  <si>
+    <t>574896808185</t>
+  </si>
+  <si>
+    <t>789574305739</t>
+  </si>
+  <si>
+    <t>463362780000</t>
+  </si>
+  <si>
+    <t>16068674490</t>
+  </si>
+  <si>
+    <t>1301566898062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1224811599234 
+</t>
+  </si>
+  <si>
+    <t>981384007386</t>
+  </si>
+  <si>
+    <t>44311536858</t>
+  </si>
+  <si>
+    <t>42865059476</t>
+  </si>
+  <si>
+    <t>145417718969</t>
+  </si>
+  <si>
+    <t>33755492629</t>
+  </si>
+  <si>
+    <t>6578654176</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>76755298828</t>
+  </si>
+  <si>
+    <t>449501802802</t>
+  </si>
+  <si>
+    <t>62105655345</t>
+  </si>
+  <si>
+    <t>44105655345</t>
+  </si>
+  <si>
+    <t>98500000000</t>
+  </si>
+  <si>
+    <t>178990404687</t>
+  </si>
+  <si>
+    <t>31143992307</t>
+  </si>
+  <si>
+    <t>1115292567721</t>
+  </si>
+  <si>
+    <t>536592088619</t>
+  </si>
+  <si>
+    <t>1564794370523</t>
+  </si>
+  <si>
+    <t>805739011913</t>
+  </si>
+  <si>
+    <t>669350116292</t>
+  </si>
+  <si>
+    <t>351100000000</t>
+  </si>
+  <si>
+    <t>759055358610</t>
+  </si>
+  <si>
+    <t>10019335223</t>
+  </si>
+  <si>
+    <t>371227203017</t>
+  </si>
+  <si>
+    <t>350232503365</t>
+  </si>
+  <si>
+    <t>299572662928</t>
+  </si>
+  <si>
+    <t>5478740992</t>
+  </si>
+  <si>
+    <t>5378263886</t>
+  </si>
+  <si>
+    <t>44414135924</t>
+  </si>
+  <si>
+    <t>8600560555</t>
+  </si>
+  <si>
+    <t>35011839957</t>
+  </si>
+  <si>
+    <t>631</t>
+  </si>
+  <si>
+    <t>20994699652</t>
   </si>
 </sst>
 </file>
@@ -46408,12 +47620,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="7.63333333333333" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="12.25" collapsed="false"/>
-    <col min="5" max="15" customWidth="true" width="7.63333333333333" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="13.75" collapsed="false"/>
-    <col min="17" max="28" customWidth="true" width="7.63333333333333" collapsed="false"/>
+    <col min="1" max="2" customWidth="true" width="7.63333333333333" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.25" collapsed="true"/>
+    <col min="5" max="15" customWidth="true" width="7.63333333333333" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="13.75" collapsed="true"/>
+    <col min="17" max="28" customWidth="true" width="7.63333333333333" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="3:28">
@@ -48382,81 +49594,1639 @@
         <v>967</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" ht="14.25" customHeight="1" spans="3:4">
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>339</v>
+      </c>
+      <c r="B24" t="s">
+        <v>968</v>
+      </c>
+      <c r="C24" t="s">
+        <v>969</v>
+      </c>
+      <c r="D24" t="s">
+        <v>528</v>
+      </c>
+      <c r="E24" t="s">
+        <v>528</v>
+      </c>
+      <c r="F24" t="s">
+        <v>528</v>
+      </c>
+      <c r="G24" t="s">
+        <v>970</v>
+      </c>
+      <c r="H24" t="s">
+        <v>971</v>
+      </c>
+      <c r="I24" t="s">
+        <v>972</v>
+      </c>
+      <c r="J24" t="s">
+        <v>973</v>
+      </c>
+      <c r="K24" t="s">
+        <v>528</v>
+      </c>
+      <c r="L24" t="s">
+        <v>974</v>
+      </c>
+      <c r="M24" t="s">
+        <v>975</v>
+      </c>
+      <c r="N24" t="s">
+        <v>528</v>
+      </c>
+      <c r="O24" t="s">
+        <v>976</v>
+      </c>
+      <c r="P24" t="s">
+        <v>977</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>528</v>
+      </c>
+      <c r="R24" t="s">
+        <v>978</v>
+      </c>
+      <c r="S24" t="s">
+        <v>979</v>
+      </c>
+      <c r="T24" t="s">
+        <v>980</v>
+      </c>
+      <c r="U24" t="s">
+        <v>981</v>
+      </c>
+      <c r="V24" t="s">
+        <v>982</v>
+      </c>
+      <c r="W24" t="s">
+        <v>528</v>
+      </c>
+      <c r="X24" t="s">
+        <v>983</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>984</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>985</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" t="s">
+        <v>987</v>
+      </c>
+      <c r="C25" t="s">
+        <v>988</v>
+      </c>
+      <c r="D25" t="s">
+        <v>989</v>
+      </c>
+      <c r="E25" t="s">
+        <v>990</v>
+      </c>
+      <c r="F25" t="s">
+        <v>528</v>
+      </c>
+      <c r="G25" t="s">
+        <v>991</v>
+      </c>
+      <c r="H25" t="s">
+        <v>992</v>
+      </c>
+      <c r="I25" t="s">
+        <v>993</v>
+      </c>
+      <c r="J25" t="s">
+        <v>994</v>
+      </c>
+      <c r="K25" t="s">
+        <v>995</v>
+      </c>
+      <c r="L25" t="s">
+        <v>996</v>
+      </c>
+      <c r="M25" t="s">
+        <v>997</v>
+      </c>
+      <c r="N25" t="s">
+        <v>528</v>
+      </c>
+      <c r="O25" t="s">
+        <v>998</v>
+      </c>
+      <c r="P25" t="s">
+        <v>977</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>528</v>
+      </c>
+      <c r="R25" t="s">
+        <v>999</v>
+      </c>
+      <c r="S25" t="s">
+        <v>1000</v>
+      </c>
+      <c r="T25" t="s">
+        <v>1001</v>
+      </c>
+      <c r="U25" t="s">
+        <v>1002</v>
+      </c>
+      <c r="V25" t="s">
+        <v>1003</v>
+      </c>
+      <c r="W25" t="s">
+        <v>528</v>
+      </c>
+      <c r="X25" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>528</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>339</v>
+      </c>
+      <c r="B26" t="s">
+        <v>743</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F26" t="s">
+        <v>528</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1010</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J26" t="s">
+        <v>1012</v>
+      </c>
+      <c r="K26" t="s">
+        <v>528</v>
+      </c>
+      <c r="L26" t="s">
+        <v>1013</v>
+      </c>
+      <c r="M26" t="s">
+        <v>1014</v>
+      </c>
+      <c r="N26" t="s">
+        <v>528</v>
+      </c>
+      <c r="O26" t="s">
+        <v>1015</v>
+      </c>
+      <c r="P26" t="s">
+        <v>1016</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>528</v>
+      </c>
+      <c r="R26" t="s">
+        <v>1017</v>
+      </c>
+      <c r="S26" t="s">
+        <v>1018</v>
+      </c>
+      <c r="T26" t="s">
+        <v>1019</v>
+      </c>
+      <c r="U26" t="s">
+        <v>1020</v>
+      </c>
+      <c r="V26" t="s">
+        <v>1021</v>
+      </c>
+      <c r="W26" t="s">
+        <v>1022</v>
+      </c>
+      <c r="X26" t="s">
+        <v>1023</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>1025</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>339</v>
+      </c>
+      <c r="B27" t="s">
+        <v>767</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F27" t="s">
+        <v>528</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1032</v>
+      </c>
+      <c r="J27" t="s">
+        <v>1033</v>
+      </c>
+      <c r="K27" t="s">
+        <v>528</v>
+      </c>
+      <c r="L27" t="s">
+        <v>1034</v>
+      </c>
+      <c r="M27" t="s">
+        <v>1035</v>
+      </c>
+      <c r="N27" t="s">
+        <v>528</v>
+      </c>
+      <c r="O27" t="s">
+        <v>1036</v>
+      </c>
+      <c r="P27" t="s">
+        <v>1037</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>528</v>
+      </c>
+      <c r="R27" t="s">
+        <v>1038</v>
+      </c>
+      <c r="S27" t="s">
+        <v>1039</v>
+      </c>
+      <c r="T27" t="s">
+        <v>1040</v>
+      </c>
+      <c r="U27" t="s">
+        <v>1041</v>
+      </c>
+      <c r="V27" t="s">
+        <v>1042</v>
+      </c>
+      <c r="W27" t="s">
+        <v>1043</v>
+      </c>
+      <c r="X27" t="s">
+        <v>1044</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>1046</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>339</v>
+      </c>
+      <c r="B28" t="s">
+        <v>790</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F28" t="s">
+        <v>528</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1054</v>
+      </c>
+      <c r="K28" t="s">
+        <v>528</v>
+      </c>
+      <c r="L28" t="s">
+        <v>1055</v>
+      </c>
+      <c r="M28" t="s">
+        <v>1056</v>
+      </c>
+      <c r="N28" t="s">
+        <v>528</v>
+      </c>
+      <c r="O28" t="s">
+        <v>1057</v>
+      </c>
+      <c r="P28" t="s">
+        <v>1058</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>528</v>
+      </c>
+      <c r="R28" t="s">
+        <v>1059</v>
+      </c>
+      <c r="S28" t="s">
+        <v>1060</v>
+      </c>
+      <c r="T28" t="s">
+        <v>1061</v>
+      </c>
+      <c r="U28" t="s">
+        <v>1062</v>
+      </c>
+      <c r="V28" t="s">
+        <v>1063</v>
+      </c>
+      <c r="W28" t="s">
+        <v>1064</v>
+      </c>
+      <c r="X28" t="s">
+        <v>1065</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>1066</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>1067</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>339</v>
+      </c>
+      <c r="B29" t="s">
+        <v>524</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1076</v>
+      </c>
+      <c r="K29" t="s">
+        <v>528</v>
+      </c>
+      <c r="L29" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M29" t="s">
+        <v>1078</v>
+      </c>
+      <c r="N29" t="s">
+        <v>528</v>
+      </c>
+      <c r="O29" t="s">
+        <v>1079</v>
+      </c>
+      <c r="P29" t="s">
+        <v>1080</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>528</v>
+      </c>
+      <c r="R29" t="s">
+        <v>1081</v>
+      </c>
+      <c r="S29" t="s">
+        <v>1082</v>
+      </c>
+      <c r="T29" t="s">
+        <v>1083</v>
+      </c>
+      <c r="U29" t="s">
+        <v>1084</v>
+      </c>
+      <c r="V29" t="s">
+        <v>1085</v>
+      </c>
+      <c r="W29" t="s">
+        <v>1086</v>
+      </c>
+      <c r="X29" t="s">
+        <v>1087</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>1088</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>1089</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>1090</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>339</v>
+      </c>
+      <c r="B30" t="s">
+        <v>548</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F30" t="s">
+        <v>528</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1095</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1098</v>
+      </c>
+      <c r="K30" t="s">
+        <v>528</v>
+      </c>
+      <c r="L30" t="s">
+        <v>1099</v>
+      </c>
+      <c r="M30" t="s">
+        <v>1100</v>
+      </c>
+      <c r="N30" t="s">
+        <v>528</v>
+      </c>
+      <c r="O30" t="s">
+        <v>1101</v>
+      </c>
+      <c r="P30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>528</v>
+      </c>
+      <c r="R30" t="s">
+        <v>1103</v>
+      </c>
+      <c r="S30" t="s">
+        <v>1104</v>
+      </c>
+      <c r="T30" t="s">
+        <v>1105</v>
+      </c>
+      <c r="U30" t="s">
+        <v>1106</v>
+      </c>
+      <c r="V30" t="s">
+        <v>1107</v>
+      </c>
+      <c r="W30" t="s">
+        <v>528</v>
+      </c>
+      <c r="X30" t="s">
+        <v>1108</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>1109</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>1110</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>1111</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>339</v>
+      </c>
+      <c r="B31" t="s">
+        <v>592</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1115</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1116</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1117</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J31" t="s">
+        <v>1119</v>
+      </c>
+      <c r="K31" t="s">
+        <v>528</v>
+      </c>
+      <c r="L31" t="s">
+        <v>1120</v>
+      </c>
+      <c r="M31" t="s">
+        <v>1121</v>
+      </c>
+      <c r="N31" t="s">
+        <v>528</v>
+      </c>
+      <c r="O31" t="s">
+        <v>1122</v>
+      </c>
+      <c r="P31" t="s">
+        <v>1123</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>528</v>
+      </c>
+      <c r="R31" t="s">
+        <v>1124</v>
+      </c>
+      <c r="S31" t="s">
+        <v>1125</v>
+      </c>
+      <c r="T31" t="s">
+        <v>1126</v>
+      </c>
+      <c r="U31" t="s">
+        <v>1127</v>
+      </c>
+      <c r="V31" t="s">
+        <v>1128</v>
+      </c>
+      <c r="W31" t="s">
+        <v>528</v>
+      </c>
+      <c r="X31" t="s">
+        <v>1129</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>1130</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>1131</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>339</v>
+      </c>
+      <c r="B32" t="s">
+        <v>633</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1139</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1140</v>
+      </c>
+      <c r="J32" t="s">
+        <v>528</v>
+      </c>
+      <c r="K32" t="s">
+        <v>1141</v>
+      </c>
+      <c r="L32" t="s">
+        <v>1142</v>
+      </c>
+      <c r="M32" t="s">
+        <v>1143</v>
+      </c>
+      <c r="N32" t="s">
+        <v>528</v>
+      </c>
+      <c r="O32" t="s">
+        <v>1144</v>
+      </c>
+      <c r="P32" t="s">
+        <v>1145</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>528</v>
+      </c>
+      <c r="R32" t="s">
+        <v>1146</v>
+      </c>
+      <c r="S32" t="s">
+        <v>1147</v>
+      </c>
+      <c r="T32" t="s">
+        <v>1148</v>
+      </c>
+      <c r="U32" t="s">
+        <v>1149</v>
+      </c>
+      <c r="V32" t="s">
+        <v>1150</v>
+      </c>
+      <c r="W32" t="s">
+        <v>528</v>
+      </c>
+      <c r="X32" t="s">
+        <v>1151</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>1152</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>1153</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B33" t="s">
+        <v>678</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F33" t="s">
+        <v>528</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1158</v>
+      </c>
+      <c r="H33" t="s">
+        <v>1159</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1160</v>
+      </c>
+      <c r="J33" t="s">
+        <v>1161</v>
+      </c>
+      <c r="K33" t="s">
+        <v>1162</v>
+      </c>
+      <c r="L33" t="s">
+        <v>1163</v>
+      </c>
+      <c r="M33" t="s">
+        <v>1164</v>
+      </c>
+      <c r="N33" t="s">
+        <v>528</v>
+      </c>
+      <c r="O33" t="s">
+        <v>1165</v>
+      </c>
+      <c r="P33" t="s">
+        <v>1145</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>528</v>
+      </c>
+      <c r="R33" t="s">
+        <v>1166</v>
+      </c>
+      <c r="S33" t="s">
+        <v>1167</v>
+      </c>
+      <c r="T33" t="s">
+        <v>1168</v>
+      </c>
+      <c r="U33" t="s">
+        <v>1169</v>
+      </c>
+      <c r="V33" t="s">
+        <v>1170</v>
+      </c>
+      <c r="W33" t="s">
+        <v>1171</v>
+      </c>
+      <c r="X33" t="s">
+        <v>1172</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>1173</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>1174</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>1175</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>339</v>
+      </c>
+      <c r="B34" t="s">
+        <v>698</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D34" t="s">
+        <v>528</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F34" t="s">
+        <v>528</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1179</v>
+      </c>
+      <c r="H34" t="s">
+        <v>528</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1180</v>
+      </c>
+      <c r="J34" t="s">
+        <v>528</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1181</v>
+      </c>
+      <c r="L34" t="s">
+        <v>1182</v>
+      </c>
+      <c r="M34" t="s">
+        <v>1183</v>
+      </c>
+      <c r="N34" t="s">
+        <v>1184</v>
+      </c>
+      <c r="O34" t="s">
+        <v>1185</v>
+      </c>
+      <c r="P34" t="s">
+        <v>1186</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>528</v>
+      </c>
+      <c r="R34" t="s">
+        <v>1187</v>
+      </c>
+      <c r="S34" t="s">
+        <v>1188</v>
+      </c>
+      <c r="T34" t="s">
+        <v>1189</v>
+      </c>
+      <c r="U34" t="s">
+        <v>1190</v>
+      </c>
+      <c r="V34" t="s">
+        <v>1191</v>
+      </c>
+      <c r="W34" t="s">
+        <v>1192</v>
+      </c>
+      <c r="X34" t="s">
+        <v>1193</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>1194</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>1195</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>1196</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>339</v>
+      </c>
+      <c r="B35" t="s">
+        <v>720</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1199</v>
+      </c>
+      <c r="F35" t="s">
+        <v>528</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1200</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1201</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1202</v>
+      </c>
+      <c r="J35" t="s">
+        <v>1203</v>
+      </c>
+      <c r="K35" t="s">
+        <v>1204</v>
+      </c>
+      <c r="L35" t="s">
+        <v>1205</v>
+      </c>
+      <c r="M35" t="s">
+        <v>1206</v>
+      </c>
+      <c r="N35" t="s">
+        <v>1207</v>
+      </c>
+      <c r="O35" t="s">
+        <v>1208</v>
+      </c>
+      <c r="P35" t="s">
+        <v>1145</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>528</v>
+      </c>
+      <c r="R35" t="s">
+        <v>1209</v>
+      </c>
+      <c r="S35" t="s">
+        <v>1210</v>
+      </c>
+      <c r="T35" t="s">
+        <v>1211</v>
+      </c>
+      <c r="U35" t="s">
+        <v>1212</v>
+      </c>
+      <c r="V35" t="s">
+        <v>528</v>
+      </c>
+      <c r="W35" t="s">
+        <v>1213</v>
+      </c>
+      <c r="X35" t="s">
+        <v>528</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>528</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>1214</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>1215</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>340</v>
+      </c>
+      <c r="B36" t="s">
+        <v>524</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F36" t="s">
+        <v>528</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1220</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1221</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1222</v>
+      </c>
+      <c r="K36" t="s">
+        <v>528</v>
+      </c>
+      <c r="L36" t="s">
+        <v>1223</v>
+      </c>
+      <c r="M36" t="s">
+        <v>1224</v>
+      </c>
+      <c r="N36" t="s">
+        <v>1225</v>
+      </c>
+      <c r="O36" t="s">
+        <v>1226</v>
+      </c>
+      <c r="P36" t="s">
+        <v>1227</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>528</v>
+      </c>
+      <c r="R36" t="s">
+        <v>1228</v>
+      </c>
+      <c r="S36" t="s">
+        <v>1229</v>
+      </c>
+      <c r="T36" t="s">
+        <v>1230</v>
+      </c>
+      <c r="U36" t="s">
+        <v>1231</v>
+      </c>
+      <c r="V36" t="s">
+        <v>1232</v>
+      </c>
+      <c r="W36" t="s">
+        <v>1232</v>
+      </c>
+      <c r="X36" t="s">
+        <v>1233</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>1234</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>1236</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>340</v>
+      </c>
+      <c r="B37" t="s">
+        <v>548</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1240</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1241</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1243</v>
+      </c>
+      <c r="J37" t="s">
+        <v>1244</v>
+      </c>
+      <c r="K37" t="s">
+        <v>528</v>
+      </c>
+      <c r="L37" t="s">
+        <v>1245</v>
+      </c>
+      <c r="M37" t="s">
+        <v>1246</v>
+      </c>
+      <c r="N37" t="s">
+        <v>1247</v>
+      </c>
+      <c r="O37" t="s">
+        <v>1248</v>
+      </c>
+      <c r="P37" t="s">
+        <v>1249</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>528</v>
+      </c>
+      <c r="R37" t="s">
+        <v>1250</v>
+      </c>
+      <c r="S37" t="s">
+        <v>1251</v>
+      </c>
+      <c r="T37" t="s">
+        <v>1252</v>
+      </c>
+      <c r="U37" t="s">
+        <v>1253</v>
+      </c>
+      <c r="V37" t="s">
+        <v>1254</v>
+      </c>
+      <c r="W37" t="s">
+        <v>1255</v>
+      </c>
+      <c r="X37" t="s">
+        <v>1256</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>1257</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>1258</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>1259</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>340</v>
+      </c>
+      <c r="B38" t="s">
+        <v>592</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1262</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1263</v>
+      </c>
+      <c r="F38" t="s">
+        <v>528</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1264</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I38" t="s">
+        <v>1266</v>
+      </c>
+      <c r="J38" t="s">
+        <v>1267</v>
+      </c>
+      <c r="K38" t="s">
+        <v>528</v>
+      </c>
+      <c r="L38" t="s">
+        <v>1268</v>
+      </c>
+      <c r="M38" t="s">
+        <v>1269</v>
+      </c>
+      <c r="N38" t="s">
+        <v>1270</v>
+      </c>
+      <c r="O38" t="s">
+        <v>1271</v>
+      </c>
+      <c r="P38" t="s">
+        <v>1249</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>528</v>
+      </c>
+      <c r="R38" t="s">
+        <v>1272</v>
+      </c>
+      <c r="S38" t="s">
+        <v>1273</v>
+      </c>
+      <c r="T38" t="s">
+        <v>1274</v>
+      </c>
+      <c r="U38" t="s">
+        <v>1275</v>
+      </c>
+      <c r="V38" t="s">
+        <v>1276</v>
+      </c>
+      <c r="W38" t="s">
+        <v>1277</v>
+      </c>
+      <c r="X38" t="s">
+        <v>1278</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>1279</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>528</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>1280</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>340</v>
+      </c>
+      <c r="B39" t="s">
+        <v>633</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1283</v>
+      </c>
+      <c r="F39" t="s">
+        <v>547</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H39" t="s">
+        <v>1285</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J39" t="s">
+        <v>1287</v>
+      </c>
+      <c r="K39" t="s">
+        <v>528</v>
+      </c>
+      <c r="L39" t="s">
+        <v>1288</v>
+      </c>
+      <c r="M39" t="s">
+        <v>1289</v>
+      </c>
+      <c r="N39" t="s">
+        <v>1290</v>
+      </c>
+      <c r="O39" t="s">
+        <v>1291</v>
+      </c>
+      <c r="P39" t="s">
+        <v>1292</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>528</v>
+      </c>
+      <c r="R39" t="s">
+        <v>528</v>
+      </c>
+      <c r="S39" t="s">
+        <v>1293</v>
+      </c>
+      <c r="T39" t="s">
+        <v>1294</v>
+      </c>
+      <c r="U39" t="s">
+        <v>1295</v>
+      </c>
+      <c r="V39" t="s">
+        <v>1296</v>
+      </c>
+      <c r="W39" t="s">
+        <v>1297</v>
+      </c>
+      <c r="X39" t="s">
+        <v>1298</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>1299</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>1300</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>1301</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>340</v>
+      </c>
+      <c r="B40" t="s">
+        <v>678</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F40" t="s">
+        <v>547</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1305</v>
+      </c>
+      <c r="H40" t="s">
+        <v>1306</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1307</v>
+      </c>
+      <c r="J40" t="s">
+        <v>1308</v>
+      </c>
+      <c r="K40" t="s">
+        <v>528</v>
+      </c>
+      <c r="L40" t="s">
+        <v>1309</v>
+      </c>
+      <c r="M40" t="s">
+        <v>1310</v>
+      </c>
+      <c r="N40" t="s">
+        <v>1311</v>
+      </c>
+      <c r="O40" t="s">
+        <v>1312</v>
+      </c>
+      <c r="P40" t="s">
+        <v>1313</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>528</v>
+      </c>
+      <c r="R40" t="s">
+        <v>1314</v>
+      </c>
+      <c r="S40" t="s">
+        <v>1315</v>
+      </c>
+      <c r="T40" t="s">
+        <v>1316</v>
+      </c>
+      <c r="U40" t="s">
+        <v>1317</v>
+      </c>
+      <c r="V40" t="s">
+        <v>1318</v>
+      </c>
+      <c r="W40" t="s">
+        <v>1319</v>
+      </c>
+      <c r="X40" t="s">
+        <v>1320</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>1321</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>1322</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>1323</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>340</v>
+      </c>
+      <c r="B41" t="s">
+        <v>698</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1326</v>
+      </c>
+      <c r="F41" t="s">
+        <v>547</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1327</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1328</v>
+      </c>
+      <c r="I41" t="s">
+        <v>1329</v>
+      </c>
+      <c r="J41" t="s">
+        <v>1330</v>
+      </c>
+      <c r="K41" t="s">
+        <v>528</v>
+      </c>
+      <c r="L41" t="s">
+        <v>1331</v>
+      </c>
+      <c r="M41" t="s">
+        <v>1332</v>
+      </c>
+      <c r="N41" t="s">
+        <v>1080</v>
+      </c>
+      <c r="O41" t="s">
+        <v>1333</v>
+      </c>
+      <c r="P41" t="s">
+        <v>1334</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>1335</v>
+      </c>
+      <c r="R41" t="s">
+        <v>528</v>
+      </c>
+      <c r="S41" t="s">
+        <v>1336</v>
+      </c>
+      <c r="T41" t="s">
+        <v>1337</v>
+      </c>
+      <c r="U41" t="s">
+        <v>1338</v>
+      </c>
+      <c r="V41" t="s">
+        <v>1339</v>
+      </c>
+      <c r="W41" t="s">
+        <v>1340</v>
+      </c>
+      <c r="X41" t="s">
+        <v>1341</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>1342</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>1343</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>1344</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>340</v>
+      </c>
+      <c r="B42" t="s">
+        <v>720</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1348</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1349</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1350</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1351</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1352</v>
+      </c>
+      <c r="J42" t="s">
+        <v>1353</v>
+      </c>
+      <c r="K42" t="s">
+        <v>1354</v>
+      </c>
+      <c r="L42" t="s">
+        <v>1355</v>
+      </c>
+      <c r="M42" t="s">
+        <v>1356</v>
+      </c>
+      <c r="N42" t="s">
+        <v>1357</v>
+      </c>
+      <c r="O42" t="s">
+        <v>1358</v>
+      </c>
+      <c r="P42" t="s">
+        <v>1334</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>528</v>
+      </c>
+      <c r="R42" t="s">
+        <v>1359</v>
+      </c>
+      <c r="S42" t="s">
+        <v>1360</v>
+      </c>
+      <c r="T42" t="s">
+        <v>1361</v>
+      </c>
+      <c r="U42" t="s">
+        <v>1362</v>
+      </c>
+      <c r="V42" t="s">
+        <v>1363</v>
+      </c>
+      <c r="W42" t="s">
+        <v>1364</v>
+      </c>
+      <c r="X42" t="s">
+        <v>1365</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>1366</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>1367</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>1368</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>1369</v>
+      </c>
     </row>
     <row r="43" ht="14.25" customHeight="1" spans="3:4">
       <c r="C43" s="5"/>

</xml_diff>

<commit_message>
Keep parentheses in original file
</commit_message>
<xml_diff>
--- a/financial_data/result.xlsx
+++ b/financial_data/result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4268" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="1369">
   <si>
     <t>Mô ta biến:</t>
   </si>
@@ -1638,19 +1638,19 @@
     <t>32325289788</t>
   </si>
   <si>
-    <t>24326263459</t>
-  </si>
-  <si>
-    <t>211844415</t>
-  </si>
-  <si>
-    <t>153432107</t>
-  </si>
-  <si>
-    <t>2253386923</t>
-  </si>
-  <si>
-    <t>6162683324</t>
+    <t>(24326263459)</t>
+  </si>
+  <si>
+    <t>(211844415)</t>
+  </si>
+  <si>
+    <t>(153432107)</t>
+  </si>
+  <si>
+    <t>(2253386923)</t>
+  </si>
+  <si>
+    <t>(6162683324)</t>
   </si>
   <si>
     <t>1313814322</t>
@@ -1707,25 +1707,25 @@
     <t>128420053151</t>
   </si>
   <si>
-    <t>107607509664</t>
-  </si>
-  <si>
-    <t>5839570743</t>
-  </si>
-  <si>
-    <t>5523770801</t>
-  </si>
-  <si>
-    <t>4040776818</t>
-  </si>
-  <si>
-    <t>4494284727</t>
+    <t>(107607509664)</t>
+  </si>
+  <si>
+    <t>(5839570743)</t>
+  </si>
+  <si>
+    <t>(5523770801)</t>
+  </si>
+  <si>
+    <t>(4040776818)</t>
+  </si>
+  <si>
+    <t>(4494284727)</t>
   </si>
   <si>
     <t>7588348790</t>
   </si>
   <si>
-    <t>5803270442</t>
+    <t>(5803270442)</t>
   </si>
   <si>
     <t>062017</t>
@@ -1776,19 +1776,19 @@
     <t>144672503033</t>
   </si>
   <si>
-    <t>103504459887</t>
-  </si>
-  <si>
-    <t>7131630201</t>
-  </si>
-  <si>
-    <t>7092126649</t>
-  </si>
-  <si>
-    <t>7205526050</t>
-  </si>
-  <si>
-    <t>2193575345</t>
+    <t>(103504459887)</t>
+  </si>
+  <si>
+    <t>(7131630201)</t>
+  </si>
+  <si>
+    <t>(7092126649)</t>
+  </si>
+  <si>
+    <t>(7205526050)</t>
+  </si>
+  <si>
+    <t>(2193575345)</t>
   </si>
   <si>
     <t>2237</t>
@@ -2451,7 +2451,7 @@
     <t>833513259394</t>
   </si>
   <si>
-    <t>9088410672</t>
+    <t>(9088410672)</t>
   </si>
   <si>
     <t>5404752006264</t>
@@ -2963,13 +2963,13 @@
     <t>780739788443</t>
   </si>
   <si>
-    <t>473477940816</t>
-  </si>
-  <si>
-    <t>46084766631</t>
-  </si>
-  <si>
-    <t>22488640000</t>
+    <t>(473477940816)</t>
+  </si>
+  <si>
+    <t>(46084766631)</t>
+  </si>
+  <si>
+    <t>(22488640000)</t>
   </si>
   <si>
     <t>81577608848</t>
@@ -2978,7 +2978,7 @@
     <t>9597</t>
   </si>
   <si>
-    <t>11447049334</t>
+    <t>(11447049334)</t>
   </si>
   <si>
     <t>122011</t>
@@ -3026,19 +3026,19 @@
     <t>851234055137</t>
   </si>
   <si>
-    <t>407262447052</t>
-  </si>
-  <si>
-    <t>49843118503</t>
-  </si>
-  <si>
-    <t>34411910765</t>
+    <t>(407262447052)</t>
+  </si>
+  <si>
+    <t>(49843118503)</t>
+  </si>
+  <si>
+    <t>(34411910765)</t>
   </si>
   <si>
     <t>96696937650</t>
   </si>
   <si>
-    <t>16827714415</t>
+    <t>(16827714415)</t>
   </si>
   <si>
     <t>752730495991</t>
@@ -3080,16 +3080,16 @@
     <t>1010693544332</t>
   </si>
   <si>
-    <t>486159567797</t>
-  </si>
-  <si>
-    <t>44142541838</t>
+    <t>(486159567797)</t>
+  </si>
+  <si>
+    <t>(44142541838)</t>
   </si>
   <si>
     <t>42053632256</t>
   </si>
   <si>
-    <t>48253324733</t>
+    <t>(48253324733)</t>
   </si>
   <si>
     <t>122677281125</t>
@@ -3098,7 +3098,7 @@
     <t>14140</t>
   </si>
   <si>
-    <t>13307605234</t>
+    <t>(13307605234)</t>
   </si>
   <si>
     <t>847434432294</t>
@@ -3143,16 +3143,16 @@
     <t>1188030523144</t>
   </si>
   <si>
-    <t>572788750670</t>
-  </si>
-  <si>
-    <t>30073766663</t>
-  </si>
-  <si>
-    <t>23630618885</t>
-  </si>
-  <si>
-    <t>43353432928</t>
+    <t>(572788750670)</t>
+  </si>
+  <si>
+    <t>(30073766663)</t>
+  </si>
+  <si>
+    <t>(23630618885)</t>
+  </si>
+  <si>
+    <t>(43353432928)</t>
   </si>
   <si>
     <t>148460241173</t>
@@ -3161,7 +3161,7 @@
     <t>15738</t>
   </si>
   <si>
-    <t>19774831983</t>
+    <t>(19774831983)</t>
   </si>
   <si>
     <t>919606072423</t>
@@ -3206,16 +3206,16 @@
     <t>1148558662932</t>
   </si>
   <si>
-    <t>581197580573</t>
-  </si>
-  <si>
-    <t>10143169581</t>
-  </si>
-  <si>
-    <t>4659667520</t>
-  </si>
-  <si>
-    <t>41928992467</t>
+    <t>(581197580573)</t>
+  </si>
+  <si>
+    <t>(10143169581)</t>
+  </si>
+  <si>
+    <t>(4659667520)</t>
+  </si>
+  <si>
+    <t>(41928992467)</t>
   </si>
   <si>
     <t>148149853143</t>
@@ -3224,7 +3224,7 @@
     <t>7792</t>
   </si>
   <si>
-    <t>23439989404</t>
+    <t>(23439989404)</t>
   </si>
   <si>
     <t>1007147961001</t>
@@ -3274,28 +3274,25 @@
     <t>1308505542154</t>
   </si>
   <si>
-    <t>684357451795</t>
-  </si>
-  <si>
-    <t>8944233426</t>
-  </si>
-  <si>
-    <t>2157000000</t>
-  </si>
-  <si>
-    <t>349298260913</t>
-  </si>
-  <si>
-    <t>41312821481</t>
+    <t>(684357451795)</t>
+  </si>
+  <si>
+    <t>(8944233426)</t>
+  </si>
+  <si>
+    <t>(2157000000)</t>
+  </si>
+  <si>
+    <t>(349298260913)</t>
+  </si>
+  <si>
+    <t>(41312821481)</t>
   </si>
   <si>
     <t>183612527947</t>
   </si>
   <si>
-    <t>5680 DN:4409</t>
-  </si>
-  <si>
-    <t>36299855165</t>
+    <t>(36299855165)</t>
   </si>
   <si>
     <t>1253811555161</t>
@@ -3340,16 +3337,16 @@
     <t>1507961143465</t>
   </si>
   <si>
-    <t>788187698499</t>
-  </si>
-  <si>
-    <t>7639010683</t>
-  </si>
-  <si>
-    <t>386019190335</t>
-  </si>
-  <si>
-    <t>50119170665</t>
+    <t>(788187698499)</t>
+  </si>
+  <si>
+    <t>(7639010683)</t>
+  </si>
+  <si>
+    <t>(386019190335)</t>
+  </si>
+  <si>
+    <t>(50119170665)</t>
   </si>
   <si>
     <t>239258578665</t>
@@ -3358,7 +3355,7 @@
     <t>5136</t>
   </si>
   <si>
-    <t>30318730277</t>
+    <t>(30318730277)</t>
   </si>
   <si>
     <t>1597850438405</t>
@@ -3403,16 +3400,16 @@
     <t>1622353239322</t>
   </si>
   <si>
-    <t>841736445654</t>
-  </si>
-  <si>
-    <t>8113705428</t>
-  </si>
-  <si>
-    <t>396533258294</t>
-  </si>
-  <si>
-    <t>54057372527</t>
+    <t>(841736445654)</t>
+  </si>
+  <si>
+    <t>(8113705428)</t>
+  </si>
+  <si>
+    <t>(396533258294)</t>
+  </si>
+  <si>
+    <t>(54057372527)</t>
   </si>
   <si>
     <t>286431011964</t>
@@ -3421,7 +3418,7 @@
     <t>4984</t>
   </si>
   <si>
-    <t>32755455122</t>
+    <t>(32755455122)</t>
   </si>
   <si>
     <t>1711319846321</t>
@@ -3469,17 +3466,17 @@
     <t>1674848940759</t>
   </si>
   <si>
-    <t>868268763818</t>
+    <t>(868268763818)</t>
   </si>
   <si>
     <t>307872357467</t>
   </si>
   <si>
-    <t>2087400000 
-391816568192</t>
-  </si>
-  <si>
-    <t>54839551083</t>
+    <t>(2087400000) 
+(391816568192)</t>
+  </si>
+  <si>
+    <t>(54839551083)</t>
   </si>
   <si>
     <t>309377697018</t>
@@ -3488,7 +3485,7 @@
     <t>4084</t>
   </si>
   <si>
-    <t>36442239366</t>
+    <t>(36442239366)</t>
   </si>
   <si>
     <t>1226340165317</t>
@@ -3530,19 +3527,19 @@
     <t>1846923436433</t>
   </si>
   <si>
-    <t>1021630484006</t>
-  </si>
-  <si>
-    <t>8678922 100</t>
-  </si>
-  <si>
-    <t>2572 798 128</t>
-  </si>
-  <si>
-    <t>363438822041</t>
-  </si>
-  <si>
-    <t>62016667072</t>
+    <t>(1021630484006)</t>
+  </si>
+  <si>
+    <t>(8678922 100)</t>
+  </si>
+  <si>
+    <t>(2572 798 128)</t>
+  </si>
+  <si>
+    <t>(363438822041)</t>
+  </si>
+  <si>
+    <t>(62016667072)</t>
   </si>
   <si>
     <t>320958930602</t>
@@ -3551,7 +3548,7 @@
     <t>4252</t>
   </si>
   <si>
-    <t>38447068590</t>
+    <t>(38447068590)</t>
   </si>
   <si>
     <t>1414546592868</t>
@@ -3593,19 +3590,19 @@
     <t>1934277133563</t>
   </si>
   <si>
-    <t>1097837462225</t>
-  </si>
-  <si>
-    <t>15577001170</t>
-  </si>
-  <si>
-    <t>9081336420</t>
-  </si>
-  <si>
-    <t>368320781916</t>
-  </si>
-  <si>
-    <t>62133020538</t>
+    <t>(1097837462225)</t>
+  </si>
+  <si>
+    <t>(15577001170)</t>
+  </si>
+  <si>
+    <t>(9081336420)</t>
+  </si>
+  <si>
+    <t>(368320781916)</t>
+  </si>
+  <si>
+    <t>(62133020538)</t>
   </si>
   <si>
     <t>317044543090</t>
@@ -3614,7 +3611,7 @@
     <t>4213</t>
   </si>
   <si>
-    <t>102520734333</t>
+    <t>(102520734333)</t>
   </si>
   <si>
     <t>1593416129655</t>
@@ -3659,10 +3656,10 @@
     <t>1076344041102</t>
   </si>
   <si>
-    <t>643009918972</t>
-  </si>
-  <si>
-    <t>5763793620</t>
+    <t>(643009918972)</t>
+  </si>
+  <si>
+    <t>(5763793620)</t>
   </si>
   <si>
     <t>164896651800</t>
@@ -3671,7 +3668,7 @@
     <t>2192</t>
   </si>
   <si>
-    <t>13411398115</t>
+    <t>(13411398115)</t>
   </si>
   <si>
     <t>142125760340</t>
@@ -4030,7 +4027,7 @@
     <t>463362780000</t>
   </si>
   <si>
-    <t>16068674490</t>
+    <t>(16068674490)</t>
   </si>
   <si>
     <t>1301566898062</t>
@@ -4103,7 +4100,7 @@
     <t>759055358610</t>
   </si>
   <si>
-    <t>10019335223</t>
+    <t>(10019335223)</t>
   </si>
   <si>
     <t>371227203017</t>
@@ -4127,10 +4124,10 @@
     <t>8600560555</t>
   </si>
   <si>
-    <t>35011839957</t>
-  </si>
-  <si>
-    <t>631</t>
+    <t>(35011839957)</t>
+  </si>
+  <si>
+    <t>(631)</t>
   </si>
   <si>
     <t>20994699652</t>
@@ -4141,10 +4138,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -4210,9 +4207,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4224,7 +4228,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4239,7 +4243,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4248,6 +4252,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4262,6 +4273,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -4270,7 +4289,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4307,16 +4326,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4331,29 +4350,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4386,7 +4383,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4398,13 +4395,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4422,7 +4437,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4434,7 +4491,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4446,127 +4551,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4632,11 +4629,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4658,9 +4676,29 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4680,200 +4718,159 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5181,11 +5178,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.75" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="36.6333333333333" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="34.75" collapsed="true"/>
-    <col min="5" max="26" customWidth="true" width="7.63333333333333" collapsed="true"/>
+    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.75" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.6333333333333" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.75" customWidth="1" collapsed="1"/>
+    <col min="5" max="26" width="7.63333333333333" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" spans="1:26">
@@ -33436,7 +33433,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" customWidth="true" width="7.63333333333333" collapsed="true"/>
+    <col min="1" max="26" width="7.63333333333333" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="1:3">
@@ -47611,21 +47608,21 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="H22" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U30" sqref="U30"/>
+      <selection pane="bottomRight" activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="7.63333333333333" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.25" collapsed="true"/>
-    <col min="5" max="15" customWidth="true" width="7.63333333333333" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="13.75" collapsed="true"/>
-    <col min="17" max="28" customWidth="true" width="7.63333333333333" collapsed="true"/>
+    <col min="1" max="2" width="7.63333333333333" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="15" width="7.63333333333333" customWidth="1"/>
+    <col min="16" max="16" width="13.75" customWidth="1"/>
+    <col min="17" max="28" width="7.63333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="3:28">
@@ -47874,7 +47871,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="13.8" spans="1:28">
       <c r="A4" t="s">
         <v>337</v>
       </c>
@@ -47960,7 +47957,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="13.8" spans="1:28">
       <c r="A5" t="s">
         <v>337</v>
       </c>
@@ -48046,7 +48043,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="13.8" spans="1:28">
       <c r="A6" t="s">
         <v>337</v>
       </c>
@@ -48132,7 +48129,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="13.8" spans="1:28">
       <c r="A7" t="s">
         <v>337</v>
       </c>
@@ -48218,7 +48215,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="13.8" spans="1:28">
       <c r="A8" t="s">
         <v>337</v>
       </c>
@@ -48304,7 +48301,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="13.8" spans="1:28">
       <c r="A9" t="s">
         <v>337</v>
       </c>
@@ -48390,7 +48387,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="13.8" spans="1:28">
       <c r="A10" t="s">
         <v>337</v>
       </c>
@@ -48476,7 +48473,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="13.8" spans="1:28">
       <c r="A11" t="s">
         <v>337</v>
       </c>
@@ -48562,7 +48559,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="13.8" spans="1:28">
       <c r="A12" t="s">
         <v>337</v>
       </c>
@@ -48648,7 +48645,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="13.8" spans="1:28">
       <c r="A13" t="s">
         <v>337</v>
       </c>
@@ -48734,7 +48731,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="13.8" spans="1:28">
       <c r="A14" t="s">
         <v>338</v>
       </c>
@@ -48820,7 +48817,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" ht="13.8" spans="1:28">
       <c r="A15" t="s">
         <v>338</v>
       </c>
@@ -48906,7 +48903,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="13.8" spans="1:28">
       <c r="A16" t="s">
         <v>338</v>
       </c>
@@ -48992,7 +48989,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="13.8" spans="1:28">
       <c r="A17" t="s">
         <v>338</v>
       </c>
@@ -49078,7 +49075,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" ht="13.8" spans="1:28">
       <c r="A18" t="s">
         <v>338</v>
       </c>
@@ -49164,7 +49161,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="13.8" spans="1:28">
       <c r="A19" t="s">
         <v>338</v>
       </c>
@@ -49250,7 +49247,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="13.8" spans="1:28">
       <c r="A20" t="s">
         <v>338</v>
       </c>
@@ -49336,7 +49333,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="13.8" spans="1:28">
       <c r="A21" t="s">
         <v>338</v>
       </c>
@@ -49422,7 +49419,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="13.8" spans="1:28">
       <c r="A22" t="s">
         <v>338</v>
       </c>
@@ -49508,7 +49505,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" ht="13.8" spans="1:28">
       <c r="A23" t="s">
         <v>338</v>
       </c>
@@ -49594,7 +49591,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" ht="13.8" spans="1:28">
       <c r="A24" t="s">
         <v>339</v>
       </c>
@@ -49680,7 +49677,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" ht="13.8" spans="1:28">
       <c r="A25" t="s">
         <v>339</v>
       </c>
@@ -49766,7 +49763,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" ht="13.8" spans="1:28">
       <c r="A26" t="s">
         <v>339</v>
       </c>
@@ -49852,7 +49849,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="13.8" spans="1:28">
       <c r="A27" t="s">
         <v>339</v>
       </c>
@@ -49938,7 +49935,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="13.8" spans="1:28">
       <c r="A28" t="s">
         <v>339</v>
       </c>
@@ -50024,7 +50021,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:28">
       <c r="A29" t="s">
         <v>339</v>
       </c>
@@ -50103,14 +50100,14 @@
       <c r="Z29" t="s">
         <v>1089</v>
       </c>
-      <c r="AA29" t="s">
+      <c r="AA29">
+        <v>5680</v>
+      </c>
+      <c r="AB29" t="s">
         <v>1090</v>
       </c>
-      <c r="AB29" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="30">
+    </row>
+    <row r="30" ht="13.8" spans="1:28">
       <c r="A30" t="s">
         <v>339</v>
       </c>
@@ -50118,85 +50115,85 @@
         <v>548</v>
       </c>
       <c r="C30" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D30" t="s">
         <v>1092</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>1093</v>
-      </c>
-      <c r="E30" t="s">
-        <v>1094</v>
       </c>
       <c r="F30" t="s">
         <v>528</v>
       </c>
       <c r="G30" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H30" t="s">
         <v>1095</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>1096</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>1097</v>
-      </c>
-      <c r="J30" t="s">
-        <v>1098</v>
       </c>
       <c r="K30" t="s">
         <v>528</v>
       </c>
       <c r="L30" t="s">
+        <v>1098</v>
+      </c>
+      <c r="M30" t="s">
         <v>1099</v>
-      </c>
-      <c r="M30" t="s">
-        <v>1100</v>
       </c>
       <c r="N30" t="s">
         <v>528</v>
       </c>
       <c r="O30" t="s">
+        <v>1100</v>
+      </c>
+      <c r="P30" t="s">
         <v>1101</v>
-      </c>
-      <c r="P30" t="s">
-        <v>1102</v>
       </c>
       <c r="Q30" t="s">
         <v>528</v>
       </c>
       <c r="R30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="S30" t="s">
         <v>1103</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>1104</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>1105</v>
       </c>
-      <c r="U30" t="s">
+      <c r="V30" t="s">
         <v>1106</v>
-      </c>
-      <c r="V30" t="s">
-        <v>1107</v>
       </c>
       <c r="W30" t="s">
         <v>528</v>
       </c>
       <c r="X30" t="s">
+        <v>1107</v>
+      </c>
+      <c r="Y30" t="s">
         <v>1108</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>1109</v>
       </c>
-      <c r="Z30" t="s">
+      <c r="AA30" t="s">
         <v>1110</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AB30" t="s">
         <v>1111</v>
       </c>
-      <c r="AB30" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="31">
+    </row>
+    <row r="31" ht="13.8" spans="1:28">
       <c r="A31" t="s">
         <v>339</v>
       </c>
@@ -50204,85 +50201,85 @@
         <v>592</v>
       </c>
       <c r="C31" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D31" t="s">
         <v>1113</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>1113</v>
+      </c>
+      <c r="F31" t="s">
         <v>1114</v>
       </c>
-      <c r="E31" t="s">
-        <v>1114</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>1115</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>1116</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>1117</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>1118</v>
-      </c>
-      <c r="J31" t="s">
-        <v>1119</v>
       </c>
       <c r="K31" t="s">
         <v>528</v>
       </c>
       <c r="L31" t="s">
+        <v>1119</v>
+      </c>
+      <c r="M31" t="s">
         <v>1120</v>
-      </c>
-      <c r="M31" t="s">
-        <v>1121</v>
       </c>
       <c r="N31" t="s">
         <v>528</v>
       </c>
       <c r="O31" t="s">
+        <v>1121</v>
+      </c>
+      <c r="P31" t="s">
         <v>1122</v>
-      </c>
-      <c r="P31" t="s">
-        <v>1123</v>
       </c>
       <c r="Q31" t="s">
         <v>528</v>
       </c>
       <c r="R31" t="s">
+        <v>1123</v>
+      </c>
+      <c r="S31" t="s">
         <v>1124</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>1125</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>1126</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>1127</v>
-      </c>
-      <c r="V31" t="s">
-        <v>1128</v>
       </c>
       <c r="W31" t="s">
         <v>528</v>
       </c>
       <c r="X31" t="s">
+        <v>1128</v>
+      </c>
+      <c r="Y31" t="s">
         <v>1129</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>1130</v>
       </c>
-      <c r="Z31" t="s">
+      <c r="AA31" t="s">
         <v>1131</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AB31" t="s">
         <v>1132</v>
       </c>
-      <c r="AB31" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="32">
+    </row>
+    <row r="32" ht="13.8" spans="1:28">
       <c r="A32" t="s">
         <v>339</v>
       </c>
@@ -50290,85 +50287,85 @@
         <v>633</v>
       </c>
       <c r="C32" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D32" t="s">
         <v>1134</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>1135</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>1136</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>1137</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>1138</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>1139</v>
-      </c>
-      <c r="I32" t="s">
-        <v>1140</v>
       </c>
       <c r="J32" t="s">
         <v>528</v>
       </c>
       <c r="K32" t="s">
+        <v>1140</v>
+      </c>
+      <c r="L32" t="s">
         <v>1141</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>1142</v>
-      </c>
-      <c r="M32" t="s">
-        <v>1143</v>
       </c>
       <c r="N32" t="s">
         <v>528</v>
       </c>
       <c r="O32" t="s">
+        <v>1143</v>
+      </c>
+      <c r="P32" t="s">
         <v>1144</v>
-      </c>
-      <c r="P32" t="s">
-        <v>1145</v>
       </c>
       <c r="Q32" t="s">
         <v>528</v>
       </c>
       <c r="R32" t="s">
+        <v>1145</v>
+      </c>
+      <c r="S32" t="s">
         <v>1146</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>1147</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>1148</v>
       </c>
-      <c r="U32" t="s">
+      <c r="V32" t="s">
         <v>1149</v>
-      </c>
-      <c r="V32" t="s">
-        <v>1150</v>
       </c>
       <c r="W32" t="s">
         <v>528</v>
       </c>
       <c r="X32" t="s">
+        <v>1150</v>
+      </c>
+      <c r="Y32" t="s">
         <v>1151</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>1152</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AA32" t="s">
         <v>1153</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AB32" t="s">
         <v>1154</v>
       </c>
-      <c r="AB32" t="s">
-        <v>1155</v>
-      </c>
-    </row>
-    <row r="33">
+    </row>
+    <row r="33" ht="13.8" spans="1:28">
       <c r="A33" t="s">
         <v>339</v>
       </c>
@@ -50376,85 +50373,85 @@
         <v>678</v>
       </c>
       <c r="C33" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D33" t="s">
         <v>1156</v>
       </c>
-      <c r="D33" t="s">
-        <v>1157</v>
-      </c>
       <c r="E33" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="F33" t="s">
         <v>528</v>
       </c>
       <c r="G33" t="s">
+        <v>1157</v>
+      </c>
+      <c r="H33" t="s">
         <v>1158</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>1159</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>1160</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>1161</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>1162</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>1163</v>
-      </c>
-      <c r="M33" t="s">
-        <v>1164</v>
       </c>
       <c r="N33" t="s">
         <v>528</v>
       </c>
       <c r="O33" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="P33" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="Q33" t="s">
         <v>528</v>
       </c>
       <c r="R33" t="s">
+        <v>1165</v>
+      </c>
+      <c r="S33" t="s">
         <v>1166</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>1167</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>1168</v>
       </c>
-      <c r="U33" t="s">
+      <c r="V33" t="s">
         <v>1169</v>
       </c>
-      <c r="V33" t="s">
+      <c r="W33" t="s">
         <v>1170</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
         <v>1171</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Y33" t="s">
         <v>1172</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="Z33" t="s">
         <v>1173</v>
       </c>
-      <c r="Z33" t="s">
+      <c r="AA33" t="s">
         <v>1174</v>
       </c>
-      <c r="AA33" t="s">
+      <c r="AB33" t="s">
         <v>1175</v>
       </c>
-      <c r="AB33" t="s">
-        <v>1176</v>
-      </c>
-    </row>
-    <row r="34">
+    </row>
+    <row r="34" ht="13.8" spans="1:28">
       <c r="A34" t="s">
         <v>339</v>
       </c>
@@ -50462,85 +50459,85 @@
         <v>698</v>
       </c>
       <c r="C34" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D34" t="s">
         <v>528</v>
       </c>
       <c r="E34" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F34" t="s">
         <v>528</v>
       </c>
       <c r="G34" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="H34" t="s">
         <v>528</v>
       </c>
       <c r="I34" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="J34" t="s">
         <v>528</v>
       </c>
       <c r="K34" t="s">
+        <v>1180</v>
+      </c>
+      <c r="L34" t="s">
         <v>1181</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>1182</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>1183</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>1184</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>1185</v>
-      </c>
-      <c r="P34" t="s">
-        <v>1186</v>
       </c>
       <c r="Q34" t="s">
         <v>528</v>
       </c>
       <c r="R34" t="s">
+        <v>1186</v>
+      </c>
+      <c r="S34" t="s">
         <v>1187</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>1188</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>1189</v>
       </c>
-      <c r="U34" t="s">
+      <c r="V34" t="s">
         <v>1190</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>1191</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>1192</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>1193</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Z34" t="s">
         <v>1194</v>
       </c>
-      <c r="Z34" t="s">
+      <c r="AA34" t="s">
         <v>1195</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AB34" t="s">
         <v>1196</v>
       </c>
-      <c r="AB34" t="s">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="35">
+    </row>
+    <row r="35" ht="13.8" spans="1:28">
       <c r="A35" t="s">
         <v>339</v>
       </c>
@@ -50548,67 +50545,67 @@
         <v>720</v>
       </c>
       <c r="C35" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D35" t="s">
         <v>1198</v>
       </c>
-      <c r="D35" t="s">
-        <v>1199</v>
-      </c>
       <c r="E35" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="F35" t="s">
         <v>528</v>
       </c>
       <c r="G35" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H35" t="s">
         <v>1200</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>1201</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>1202</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>1203</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>1204</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>1205</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>1206</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>1207</v>
       </c>
-      <c r="O35" t="s">
-        <v>1208</v>
-      </c>
       <c r="P35" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="Q35" t="s">
         <v>528</v>
       </c>
       <c r="R35" t="s">
+        <v>1208</v>
+      </c>
+      <c r="S35" t="s">
         <v>1209</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>1210</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>1211</v>
-      </c>
-      <c r="U35" t="s">
-        <v>1212</v>
       </c>
       <c r="V35" t="s">
         <v>528</v>
       </c>
       <c r="W35" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="X35" t="s">
         <v>528</v>
@@ -50617,16 +50614,16 @@
         <v>528</v>
       </c>
       <c r="Z35" t="s">
+        <v>1213</v>
+      </c>
+      <c r="AA35" t="s">
         <v>1214</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AB35" t="s">
         <v>1215</v>
       </c>
-      <c r="AB35" t="s">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="36">
+    </row>
+    <row r="36" ht="13.8" spans="1:28">
       <c r="A36" t="s">
         <v>340</v>
       </c>
@@ -50634,85 +50631,85 @@
         <v>524</v>
       </c>
       <c r="C36" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D36" t="s">
         <v>1217</v>
       </c>
-      <c r="D36" t="s">
-        <v>1218</v>
-      </c>
       <c r="E36" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="F36" t="s">
         <v>528</v>
       </c>
       <c r="G36" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H36" t="s">
         <v>1219</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>1220</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>1221</v>
-      </c>
-      <c r="J36" t="s">
-        <v>1222</v>
       </c>
       <c r="K36" t="s">
         <v>528</v>
       </c>
       <c r="L36" t="s">
+        <v>1222</v>
+      </c>
+      <c r="M36" t="s">
         <v>1223</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>1224</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>1225</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>1226</v>
-      </c>
-      <c r="P36" t="s">
-        <v>1227</v>
       </c>
       <c r="Q36" t="s">
         <v>528</v>
       </c>
       <c r="R36" t="s">
+        <v>1227</v>
+      </c>
+      <c r="S36" t="s">
         <v>1228</v>
       </c>
-      <c r="S36" t="s">
+      <c r="T36" t="s">
         <v>1229</v>
       </c>
-      <c r="T36" t="s">
+      <c r="U36" t="s">
         <v>1230</v>
       </c>
-      <c r="U36" t="s">
+      <c r="V36" t="s">
         <v>1231</v>
       </c>
-      <c r="V36" t="s">
+      <c r="W36" t="s">
+        <v>1231</v>
+      </c>
+      <c r="X36" t="s">
         <v>1232</v>
       </c>
-      <c r="W36" t="s">
-        <v>1232</v>
-      </c>
-      <c r="X36" t="s">
+      <c r="Y36" t="s">
         <v>1233</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Z36" t="s">
         <v>1234</v>
       </c>
-      <c r="Z36" t="s">
+      <c r="AA36" t="s">
         <v>1235</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AB36" t="s">
         <v>1236</v>
       </c>
-      <c r="AB36" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="37">
+    </row>
+    <row r="37" ht="13.8" spans="1:28">
       <c r="A37" t="s">
         <v>340</v>
       </c>
@@ -50720,85 +50717,85 @@
         <v>548</v>
       </c>
       <c r="C37" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D37" t="s">
         <v>1238</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F37" t="s">
         <v>1239</v>
       </c>
-      <c r="E37" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>1240</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>1241</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>1242</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>1243</v>
-      </c>
-      <c r="J37" t="s">
-        <v>1244</v>
       </c>
       <c r="K37" t="s">
         <v>528</v>
       </c>
       <c r="L37" t="s">
+        <v>1244</v>
+      </c>
+      <c r="M37" t="s">
         <v>1245</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>1246</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>1247</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>1248</v>
-      </c>
-      <c r="P37" t="s">
-        <v>1249</v>
       </c>
       <c r="Q37" t="s">
         <v>528</v>
       </c>
       <c r="R37" t="s">
+        <v>1249</v>
+      </c>
+      <c r="S37" t="s">
         <v>1250</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>1251</v>
       </c>
-      <c r="T37" t="s">
+      <c r="U37" t="s">
         <v>1252</v>
       </c>
-      <c r="U37" t="s">
+      <c r="V37" t="s">
         <v>1253</v>
       </c>
-      <c r="V37" t="s">
+      <c r="W37" t="s">
         <v>1254</v>
       </c>
-      <c r="W37" t="s">
+      <c r="X37" t="s">
         <v>1255</v>
       </c>
-      <c r="X37" t="s">
+      <c r="Y37" t="s">
         <v>1256</v>
       </c>
-      <c r="Y37" t="s">
+      <c r="Z37" t="s">
         <v>1257</v>
       </c>
-      <c r="Z37" t="s">
+      <c r="AA37" t="s">
         <v>1258</v>
       </c>
-      <c r="AA37" t="s">
+      <c r="AB37" t="s">
         <v>1259</v>
       </c>
-      <c r="AB37" t="s">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="38">
+    </row>
+    <row r="38" ht="13.8" spans="1:28">
       <c r="A38" t="s">
         <v>340</v>
       </c>
@@ -50806,85 +50803,85 @@
         <v>592</v>
       </c>
       <c r="C38" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D38" t="s">
         <v>1261</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>1262</v>
-      </c>
-      <c r="E38" t="s">
-        <v>1263</v>
       </c>
       <c r="F38" t="s">
         <v>528</v>
       </c>
       <c r="G38" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H38" t="s">
         <v>1264</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>1265</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>1266</v>
-      </c>
-      <c r="J38" t="s">
-        <v>1267</v>
       </c>
       <c r="K38" t="s">
         <v>528</v>
       </c>
       <c r="L38" t="s">
+        <v>1267</v>
+      </c>
+      <c r="M38" t="s">
         <v>1268</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>1269</v>
       </c>
-      <c r="N38" t="s">
+      <c r="O38" t="s">
         <v>1270</v>
       </c>
-      <c r="O38" t="s">
-        <v>1271</v>
-      </c>
       <c r="P38" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="Q38" t="s">
         <v>528</v>
       </c>
       <c r="R38" t="s">
+        <v>1271</v>
+      </c>
+      <c r="S38" t="s">
         <v>1272</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>1273</v>
       </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
         <v>1274</v>
       </c>
-      <c r="U38" t="s">
+      <c r="V38" t="s">
         <v>1275</v>
       </c>
-      <c r="V38" t="s">
+      <c r="W38" t="s">
         <v>1276</v>
       </c>
-      <c r="W38" t="s">
+      <c r="X38" t="s">
         <v>1277</v>
       </c>
-      <c r="X38" t="s">
+      <c r="Y38" t="s">
         <v>1278</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>1279</v>
       </c>
       <c r="Z38" t="s">
         <v>528</v>
       </c>
       <c r="AA38" t="s">
+        <v>1279</v>
+      </c>
+      <c r="AB38" t="s">
         <v>1280</v>
       </c>
-      <c r="AB38" t="s">
-        <v>1281</v>
-      </c>
-    </row>
-    <row r="39">
+    </row>
+    <row r="39" ht="13.8" spans="1:28">
       <c r="A39" t="s">
         <v>340</v>
       </c>
@@ -50892,46 +50889,46 @@
         <v>633</v>
       </c>
       <c r="C39" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D39" t="s">
         <v>1282</v>
       </c>
-      <c r="D39" t="s">
-        <v>1283</v>
-      </c>
       <c r="E39" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="F39" t="s">
         <v>547</v>
       </c>
       <c r="G39" t="s">
+        <v>1283</v>
+      </c>
+      <c r="H39" t="s">
         <v>1284</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>1285</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>1286</v>
-      </c>
-      <c r="J39" t="s">
-        <v>1287</v>
       </c>
       <c r="K39" t="s">
         <v>528</v>
       </c>
       <c r="L39" t="s">
+        <v>1287</v>
+      </c>
+      <c r="M39" t="s">
         <v>1288</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>1289</v>
       </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>1290</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>1291</v>
-      </c>
-      <c r="P39" t="s">
-        <v>1292</v>
       </c>
       <c r="Q39" t="s">
         <v>528</v>
@@ -50940,37 +50937,37 @@
         <v>528</v>
       </c>
       <c r="S39" t="s">
+        <v>1292</v>
+      </c>
+      <c r="T39" t="s">
         <v>1293</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
         <v>1294</v>
       </c>
-      <c r="U39" t="s">
+      <c r="V39" t="s">
         <v>1295</v>
       </c>
-      <c r="V39" t="s">
+      <c r="W39" t="s">
         <v>1296</v>
       </c>
-      <c r="W39" t="s">
+      <c r="X39" t="s">
         <v>1297</v>
       </c>
-      <c r="X39" t="s">
+      <c r="Y39" t="s">
         <v>1298</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Z39" t="s">
         <v>1299</v>
       </c>
-      <c r="Z39" t="s">
+      <c r="AA39" t="s">
         <v>1300</v>
       </c>
-      <c r="AA39" t="s">
+      <c r="AB39" t="s">
         <v>1301</v>
       </c>
-      <c r="AB39" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="40">
+    </row>
+    <row r="40" ht="13.8" spans="1:28">
       <c r="A40" t="s">
         <v>340</v>
       </c>
@@ -50978,85 +50975,85 @@
         <v>678</v>
       </c>
       <c r="C40" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D40" t="s">
         <v>1303</v>
       </c>
-      <c r="D40" t="s">
-        <v>1304</v>
-      </c>
       <c r="E40" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="F40" t="s">
         <v>547</v>
       </c>
       <c r="G40" t="s">
+        <v>1304</v>
+      </c>
+      <c r="H40" t="s">
         <v>1305</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>1306</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>1307</v>
-      </c>
-      <c r="J40" t="s">
-        <v>1308</v>
       </c>
       <c r="K40" t="s">
         <v>528</v>
       </c>
       <c r="L40" t="s">
+        <v>1308</v>
+      </c>
+      <c r="M40" t="s">
         <v>1309</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>1310</v>
       </c>
-      <c r="N40" t="s">
+      <c r="O40" t="s">
         <v>1311</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>1312</v>
-      </c>
-      <c r="P40" t="s">
-        <v>1313</v>
       </c>
       <c r="Q40" t="s">
         <v>528</v>
       </c>
       <c r="R40" t="s">
+        <v>1313</v>
+      </c>
+      <c r="S40" t="s">
         <v>1314</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>1315</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
         <v>1316</v>
       </c>
-      <c r="U40" t="s">
+      <c r="V40" t="s">
         <v>1317</v>
       </c>
-      <c r="V40" t="s">
+      <c r="W40" t="s">
         <v>1318</v>
       </c>
-      <c r="W40" t="s">
+      <c r="X40" t="s">
         <v>1319</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
         <v>1320</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>1321</v>
       </c>
-      <c r="Z40" t="s">
+      <c r="AA40" t="s">
         <v>1322</v>
       </c>
-      <c r="AA40" t="s">
+      <c r="AB40" t="s">
         <v>1323</v>
       </c>
-      <c r="AB40" t="s">
-        <v>1324</v>
-      </c>
-    </row>
-    <row r="41">
+    </row>
+    <row r="41" ht="13.8" spans="1:28">
       <c r="A41" t="s">
         <v>340</v>
       </c>
@@ -51064,85 +51061,85 @@
         <v>698</v>
       </c>
       <c r="C41" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D41" t="s">
         <v>1325</v>
       </c>
-      <c r="D41" t="s">
-        <v>1326</v>
-      </c>
       <c r="E41" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="F41" t="s">
         <v>547</v>
       </c>
       <c r="G41" t="s">
+        <v>1326</v>
+      </c>
+      <c r="H41" t="s">
         <v>1327</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>1328</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>1329</v>
-      </c>
-      <c r="J41" t="s">
-        <v>1330</v>
       </c>
       <c r="K41" t="s">
         <v>528</v>
       </c>
       <c r="L41" t="s">
+        <v>1330</v>
+      </c>
+      <c r="M41" t="s">
         <v>1331</v>
-      </c>
-      <c r="M41" t="s">
-        <v>1332</v>
       </c>
       <c r="N41" t="s">
         <v>1080</v>
       </c>
       <c r="O41" t="s">
+        <v>1332</v>
+      </c>
+      <c r="P41" t="s">
         <v>1333</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>1334</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>1335</v>
       </c>
       <c r="R41" t="s">
         <v>528</v>
       </c>
       <c r="S41" t="s">
+        <v>1335</v>
+      </c>
+      <c r="T41" t="s">
         <v>1336</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
         <v>1337</v>
       </c>
-      <c r="U41" t="s">
+      <c r="V41" t="s">
         <v>1338</v>
       </c>
-      <c r="V41" t="s">
+      <c r="W41" t="s">
         <v>1339</v>
       </c>
-      <c r="W41" t="s">
+      <c r="X41" t="s">
         <v>1340</v>
       </c>
-      <c r="X41" t="s">
+      <c r="Y41" t="s">
         <v>1341</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="Z41" t="s">
         <v>1342</v>
       </c>
-      <c r="Z41" t="s">
+      <c r="AA41" t="s">
         <v>1343</v>
       </c>
-      <c r="AA41" t="s">
+      <c r="AB41" t="s">
         <v>1344</v>
       </c>
-      <c r="AB41" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="42">
+    </row>
+    <row r="42" ht="13.8" spans="1:28">
       <c r="A42" t="s">
         <v>340</v>
       </c>
@@ -51150,82 +51147,82 @@
         <v>720</v>
       </c>
       <c r="C42" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D42" t="s">
         <v>1346</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>1347</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>1348</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>1349</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>1350</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>1351</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>1352</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>1353</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>1354</v>
       </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
         <v>1355</v>
       </c>
-      <c r="M42" t="s">
+      <c r="N42" t="s">
         <v>1356</v>
       </c>
-      <c r="N42" t="s">
+      <c r="O42" t="s">
         <v>1357</v>
       </c>
-      <c r="O42" t="s">
-        <v>1358</v>
-      </c>
       <c r="P42" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="Q42" t="s">
         <v>528</v>
       </c>
       <c r="R42" t="s">
+        <v>1358</v>
+      </c>
+      <c r="S42" t="s">
         <v>1359</v>
       </c>
-      <c r="S42" t="s">
+      <c r="T42" t="s">
         <v>1360</v>
       </c>
-      <c r="T42" t="s">
+      <c r="U42" t="s">
         <v>1361</v>
       </c>
-      <c r="U42" t="s">
+      <c r="V42" t="s">
         <v>1362</v>
       </c>
-      <c r="V42" t="s">
+      <c r="W42" t="s">
         <v>1363</v>
       </c>
-      <c r="W42" t="s">
+      <c r="X42" t="s">
         <v>1364</v>
       </c>
-      <c r="X42" t="s">
+      <c r="Y42" t="s">
         <v>1365</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>1366</v>
       </c>
-      <c r="Z42" t="s">
+      <c r="AA42" t="s">
         <v>1367</v>
       </c>
-      <c r="AA42" t="s">
+      <c r="AB42" t="s">
         <v>1368</v>
-      </c>
-      <c r="AB42" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1" spans="3:4">

</xml_diff>